<commit_message>
fix little seek and index bug
</commit_message>
<xml_diff>
--- a/tests/for_fuker.allprocess_xls/allprocess_xls_test_set_dropdown_and_ruleexamplerow.xlsx
+++ b/tests/for_fuker.allprocess_xls/allprocess_xls_test_set_dropdown_and_ruleexamplerow.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="2990" windowWidth="10800" windowHeight="7810" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="9600" yWindow="0" windowWidth="9600" windowHeight="10800" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -580,19 +580,19 @@
       <c r="E6" s="2" t="inlineStr">
         <is>
           <t>·规则：哲学,经济学,法学,教育学,文学等13个选项
-·样例：文学</t>
+·样例：艺术学</t>
         </is>
       </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
           <t>·规则：哲学,理论经济学,应用经济学,法学等111个选项
-·样例：世界史</t>
+·样例：系统科学</t>
         </is>
       </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
           <t>·规则：是,否
-·样例：是</t>
+·样例：否</t>
         </is>
       </c>
       <c r="I6" s="2" t="inlineStr">
@@ -604,25 +604,25 @@
       <c r="J6" s="2" t="inlineStr">
         <is>
           <t>·规则：北京,天津,上海,重庆,河北,山西等35个选项
-·样例：青海</t>
+·样例：天津</t>
         </is>
       </c>
       <c r="L6" s="2" t="inlineStr">
         <is>
           <t>·规则：数学科学学院,物理学院等73个选项
-·样例：燕京学堂</t>
+·样例：歌剧研究院</t>
         </is>
       </c>
       <c r="R6" s="2" t="inlineStr">
         <is>
           <t>·规则：男,女
-·样例：男</t>
+·样例：女</t>
         </is>
       </c>
       <c r="S6" s="2" t="inlineStr">
         <is>
           <t>·规则：数学科学学院,物理学院等73个选项
-·样例：教育学院</t>
+·样例：基础医学院</t>
         </is>
       </c>
     </row>

</xml_diff>